<commit_message>
Suite 30 j glissants
</commit_message>
<xml_diff>
--- a/data/Climat.xlsx
+++ b/data/Climat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clemster\Documents\Cours\EPSI_I5\Qualite_des_donnees\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clemster\Documents\Cours\EPSI_I5\Qualite_des_donnees\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0E69DC-8B06-4E29-8501-1DDC7BFBDF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23E343C-1923-4FD2-AD82-FBECDB88ED7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>janvier</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>implémenter ces lois dans votre application précédente</t>
-  </si>
-  <si>
-    <t>https://stackoverflow.com/questions/43327975/how-can-i-read-a-rangea5b10-and-place-these-values-into-a-dataframe-using-o</t>
   </si>
 </sst>
 </file>
@@ -775,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2094,9 +2091,6 @@
       </c>
       <c r="D43" t="s">
         <v>54</v>
-      </c>
-      <c r="G43" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>